<commit_message>
Сontrol files were replaced (the old ones were in English, the new ones in Danish)
- Replaced control files with Danish versions
- Fixed timeout issue when reading control files
</commit_message>
<xml_diff>
--- a/eform-client/cypress/fixtures/2021-11-01T00_00_00.000Z_2022-04-01T00_00_00.000Z_report.xlsx
+++ b/eform-client/cypress/fixtures/2021-11-01T00_00_00.000Z_2022-04-01T00_00_00.000Z_report.xlsx
@@ -6,9 +6,9 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="19 - 03. Control floating laye" sheetId="2" r:id="rId2"/>
-    <x:sheet name="23 - 04. Feeding documentation" sheetId="3" r:id="rId3"/>
-    <x:sheet name="77 - 20. Task completed" sheetId="4" r:id="rId4"/>
+    <x:sheet name="19 - 03. Kontrol flydelag" sheetId="2" r:id="rId2"/>
+    <x:sheet name="23 - 04. Foderindlægssedler" sheetId="3" r:id="rId3"/>
+    <x:sheet name="77 - 20. Arbejdsopgave udført" sheetId="4" r:id="rId4"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -21,40 +21,40 @@
     <x:t>Id</x:t>
   </x:si>
   <x:si>
-    <x:t>Property</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Created At</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Done By</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Item name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Floating layer OK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Select reason for lack of floating layer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tjørntved</x:t>
+    <x:t>Ejendom</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dato</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Udført af</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Område</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Flydelag OK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vælg årsag til manglende flydelag</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kommentar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Farm 1</x:t>
   </x:si>
   <x:si>
     <x:t>Kristian Poulsen</x:t>
   </x:si>
   <x:si>
-    <x:t>G1: Floating layer</x:t>
+    <x:t>G1: Flydelag</x:t>
   </x:si>
   <x:si>
     <x:t/>
   </x:si>
   <x:si>
-    <x:t>G2: Floating layer</x:t>
+    <x:t>G2: Flydelag</x:t>
   </x:si>
   <x:si>
     <x:t>Biskopstorp</x:t>
@@ -63,10 +63,10 @@
     <x:t>0</x:t>
   </x:si>
   <x:si>
-    <x:t>Slurry tank empty</x:t>
-  </x:si>
-  <x:si>
-    <x:t>G3: Floating layer</x:t>
+    <x:t>Beholder tom</x:t>
+  </x:si>
+  <x:si>
+    <x:t>G3: Flydelag</x:t>
   </x:si>
   <x:si>
     <x:t>Mineraler</x:t>
@@ -91,7 +91,7 @@
     <x:t>Biskopstorp (Valerii)</x:t>
   </x:si>
   <x:si>
-    <x:t>Task completed</x:t>
+    <x:t>Opgave udført</x:t>
   </x:si>
   <x:si>
     <x:t>Vask blandekar</x:t>

</xml_diff>

<commit_message>
Fixing broken report tests.
</commit_message>
<xml_diff>
--- a/eform-client/cypress/fixtures/2021-11-01T00_00_00.000Z_2022-04-01T00_00_00.000Z_report.xlsx
+++ b/eform-client/cypress/fixtures/2021-11-01T00_00_00.000Z_2022-04-01T00_00_00.000Z_report.xlsx
@@ -10,7 +10,11 @@
     <x:sheet name="23 - 04. Foderindlægssedler" sheetId="3" r:id="rId3"/>
     <x:sheet name="77 - 20. Arbejdsopgave udført" sheetId="4" r:id="rId4"/>
   </x:sheets>
-  <x:definedNames/>
+  <x:definedNames>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'19 - 03. Kontrol flydelag'!$A$1:$H$9</x:definedName>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'23 - 04. Foderindlægssedler'!$A$1:$F$30</x:definedName>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'77 - 20. Arbejdsopgave udført'!$A$1:$G$23</x:definedName>
+  </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
@@ -58,9 +62,6 @@
   </x:si>
   <x:si>
     <x:t>Biskopstorp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0</x:t>
   </x:si>
   <x:si>
     <x:t>Beholder tom</x:t>
@@ -600,11 +601,11 @@
       <x:c r="E4" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F4" s="3" t="s">
+      <x:c r="F4" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G4" s="3" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="G4" s="3" t="s">
-        <x:v>15</x:v>
       </x:c>
       <x:c r="H4" s="3" t="s">
         <x:v>11</x:v>
@@ -626,11 +627,11 @@
       <x:c r="E5" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="F5" s="3" t="s">
+      <x:c r="F5" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G5" s="3" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="G5" s="3" t="s">
-        <x:v>15</x:v>
       </x:c>
       <x:c r="H5" s="3" t="s">
         <x:v>11</x:v>
@@ -650,7 +651,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F6" s="0">
         <x:v>1</x:v>
@@ -741,6 +742,7 @@
       </x:c>
     </x:row>
   </x:sheetData>
+  <x:autoFilter ref="A1:H9"/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
@@ -794,7 +796,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F2" s="3" t="s">
         <x:v>11</x:v>
@@ -814,7 +816,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F3" s="3" t="s">
         <x:v>11</x:v>
@@ -834,7 +836,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F4" s="3" t="s">
         <x:v>11</x:v>
@@ -854,7 +856,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F5" s="3" t="s">
         <x:v>11</x:v>
@@ -874,7 +876,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F6" s="3" t="s">
         <x:v>11</x:v>
@@ -894,7 +896,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F7" s="3" t="s">
         <x:v>11</x:v>
@@ -914,7 +916,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F8" s="3" t="s">
         <x:v>11</x:v>
@@ -934,7 +936,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F9" s="3" t="s">
         <x:v>11</x:v>
@@ -954,7 +956,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F10" s="3" t="s">
         <x:v>11</x:v>
@@ -974,7 +976,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F11" s="3" t="s">
         <x:v>11</x:v>
@@ -994,7 +996,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="F12" s="3" t="s">
         <x:v>11</x:v>
@@ -1014,7 +1016,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F13" s="3" t="s">
         <x:v>11</x:v>
@@ -1034,7 +1036,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F14" s="3" t="s">
         <x:v>11</x:v>
@@ -1054,7 +1056,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F15" s="3" t="s">
         <x:v>11</x:v>
@@ -1074,10 +1076,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F16" s="4" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:6">
@@ -1094,7 +1096,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F17" s="3" t="s">
         <x:v>11</x:v>
@@ -1114,7 +1116,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F18" s="3" t="s">
         <x:v>11</x:v>
@@ -1134,7 +1136,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="F19" s="3" t="s">
         <x:v>11</x:v>
@@ -1154,7 +1156,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="F20" s="3" t="s">
         <x:v>11</x:v>
@@ -1174,7 +1176,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F21" s="3" t="s">
         <x:v>11</x:v>
@@ -1194,7 +1196,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F22" s="3" t="s">
         <x:v>11</x:v>
@@ -1214,7 +1216,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F23" s="3" t="s">
         <x:v>11</x:v>
@@ -1231,10 +1233,10 @@
         <x:v>44637.4530902778</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F24" s="3" t="s">
         <x:v>11</x:v>
@@ -1251,10 +1253,10 @@
         <x:v>44637.4552083333</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F25" s="3" t="s">
         <x:v>11</x:v>
@@ -1274,7 +1276,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F26" s="3" t="s">
         <x:v>11</x:v>
@@ -1291,10 +1293,10 @@
         <x:v>44648.361712963</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="F27" s="3" t="s">
         <x:v>11</x:v>
@@ -1314,7 +1316,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F28" s="3" t="s">
         <x:v>11</x:v>
@@ -1334,7 +1336,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F29" s="3" t="s">
         <x:v>11</x:v>
@@ -1354,13 +1356,14 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F30" s="3" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
+  <x:autoFilter ref="A1:F30"/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
@@ -1397,7 +1400,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="F1" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G1" s="1" t="s">
         <x:v>7</x:v>
@@ -1417,7 +1420,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F2" s="0">
         <x:v>1</x:v>
@@ -1440,7 +1443,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F3" s="0">
         <x:v>1</x:v>
@@ -1463,7 +1466,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F4" s="0">
         <x:v>1</x:v>
@@ -1486,7 +1489,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F5" s="0">
         <x:v>1</x:v>
@@ -1509,7 +1512,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F6" s="0">
         <x:v>1</x:v>
@@ -1532,7 +1535,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F7" s="0">
         <x:v>1</x:v>
@@ -1555,7 +1558,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F8" s="0">
         <x:v>1</x:v>
@@ -1575,10 +1578,10 @@
         <x:v>44587.4349884259</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F9" s="0">
         <x:v>1</x:v>
@@ -1598,10 +1601,10 @@
         <x:v>44595.5599421296</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F10" s="0">
         <x:v>1</x:v>
@@ -1624,7 +1627,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F11" s="0">
         <x:v>1</x:v>
@@ -1647,7 +1650,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F12" s="0">
         <x:v>1</x:v>
@@ -1667,10 +1670,10 @@
         <x:v>44617.5254050926</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="F13" s="0">
         <x:v>1</x:v>
@@ -1690,10 +1693,10 @@
         <x:v>44617.5256597222</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F14" s="0">
         <x:v>1</x:v>
@@ -1713,10 +1716,10 @@
         <x:v>44627.5952546296</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F15" s="0">
         <x:v>1</x:v>
@@ -1739,7 +1742,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F16" s="0">
         <x:v>1</x:v>
@@ -1759,10 +1762,10 @@
         <x:v>44631.4567013889</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
         <x:v>29</x:v>
-      </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>30</x:v>
       </x:c>
       <x:c r="F17" s="0">
         <x:v>1</x:v>
@@ -1782,10 +1785,10 @@
         <x:v>44638.3929976852</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F18" s="0">
         <x:v>1</x:v>
@@ -1805,10 +1808,10 @@
         <x:v>44638.3935763889</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F19" s="0">
         <x:v>1</x:v>
@@ -1828,10 +1831,10 @@
         <x:v>44641.5940509259</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
         <x:v>29</x:v>
-      </x:c>
-      <x:c r="E20" s="0" t="s">
-        <x:v>30</x:v>
       </x:c>
       <x:c r="F20" s="0">
         <x:v>1</x:v>
@@ -1854,7 +1857,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F21" s="0">
         <x:v>1</x:v>
@@ -1874,10 +1877,10 @@
         <x:v>44652.4965625</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="F22" s="0">
         <x:v>1</x:v>
@@ -1897,10 +1900,10 @@
         <x:v>44652.5067824074</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F23" s="0">
         <x:v>1</x:v>
@@ -1910,6 +1913,7 @@
       </x:c>
     </x:row>
   </x:sheetData>
+  <x:autoFilter ref="A1:G23"/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>